<commit_message>
Now accepts different but equally correct descriptors coming from the same bundle
</commit_message>
<xml_diff>
--- a/benchmarking/results/spot_Phi-3-mini-4k-instruct_ep10_training_ds_v16_3-17_1-2_param-4_05112024_eval-summary.xlsx
+++ b/benchmarking/results/spot_Phi-3-mini-4k-instruct_ep10_training_ds_v16_3-17_1-2_param-4_05112024_eval-summary.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -570,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3948717948717949</v>
+        <v>0.4</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -579,16 +579,16 @@
         <v>0.8769230769230769</v>
       </c>
       <c r="E2" t="n">
-        <v>0.676923076923077</v>
+        <v>0.6871794871794872</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8179487179487179</v>
+        <v>0.8213675213675214</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7076923076923077</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8367521367521367</v>
       </c>
       <c r="I2" t="n">
         <v>0.5223880597014925</v>
@@ -600,13 +600,13 @@
         <v>0.5621890547263682</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4090909090909091</v>
+        <v>0.4155844155844156</v>
       </c>
       <c r="M2" t="n">
         <v>41</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5971223021582733</v>
+        <v>0.6007194244604317</v>
       </c>
       <c r="O2" t="n">
         <v>0.425</v>
@@ -615,10 +615,10 @@
         <v>0.4375</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2613636363636364</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3305785123966942</v>
+        <v>0.3388429752066116</v>
       </c>
       <c r="S2" t="n">
         <v>0.4125874125874126</v>

</xml_diff>